<commit_message>
#208 Improve error handling
</commit_message>
<xml_diff>
--- a/app/data/input_format.xlsx
+++ b/app/data/input_format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
     <t>ghg_s3</t>
   </si>
   <si>
-    <t>revenu</t>
+    <t>company_revenue</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
     <tableColumn id="6" name="sector"/>
     <tableColumn id="18" name="ghg_s1s2"/>
     <tableColumn id="8" name="ghg_s3"/>
-    <tableColumn id="9" name="revenu"/>
+    <tableColumn id="9" name="company_revenue"/>
     <tableColumn id="10" name="market_cap"/>
     <tableColumn id="11" name="company_enterprise_value"/>
     <tableColumn id="12" name="company_total_assets" dataDxfId="0">
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1029,7 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="21.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
@@ -3032,8 +3032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#178 Fix revenue (should be "company_revenue")
</commit_message>
<xml_diff>
--- a/app/data/input_format.xlsx
+++ b/app/data/input_format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
     <t>ghg_s3</t>
   </si>
   <si>
-    <t>revenu</t>
+    <t>company_revenue</t>
   </si>
 </sst>
 </file>
@@ -717,7 +717,7 @@
     <tableColumn id="6" name="sector"/>
     <tableColumn id="18" name="ghg_s1s2"/>
     <tableColumn id="8" name="ghg_s3"/>
-    <tableColumn id="9" name="revenu"/>
+    <tableColumn id="9" name="company_revenue"/>
     <tableColumn id="10" name="market_cap"/>
     <tableColumn id="11" name="company_enterprise_value"/>
     <tableColumn id="12" name="company_total_assets" dataDxfId="0">
@@ -1019,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1029,7 @@
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="21.5703125" customWidth="1"/>
     <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
@@ -3032,7 +3032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#178 Fix market cap and cash equivalents
</commit_message>
<xml_diff>
--- a/app/data/input_format.xlsx
+++ b/app/data/input_format.xlsx
@@ -42,12 +42,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>market_cap</t>
-  </si>
-  <si>
-    <t>cash_equivalents</t>
-  </si>
-  <si>
     <t>Advanced Micro Devices, Inc</t>
   </si>
   <si>
@@ -595,6 +589,12 @@
   </si>
   <si>
     <t>company_revenue</t>
+  </si>
+  <si>
+    <t>company_market_cap</t>
+  </si>
+  <si>
+    <t>company_cash_equivalents</t>
   </si>
 </sst>
 </file>
@@ -718,12 +718,12 @@
     <tableColumn id="18" name="ghg_s1s2"/>
     <tableColumn id="8" name="ghg_s3"/>
     <tableColumn id="9" name="company_revenue"/>
-    <tableColumn id="10" name="market_cap"/>
+    <tableColumn id="10" name="company_market_cap"/>
     <tableColumn id="11" name="company_enterprise_value"/>
     <tableColumn id="12" name="company_total_assets" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[market_cap]]*Q3</calculatedColumnFormula>
+      <calculatedColumnFormula>Table1[[#This Row],[company_market_cap]]*Q3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="cash_equivalents"/>
+    <tableColumn id="13" name="company_cash_equivalents"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1020,7 +1020,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,69 +1066,69 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" t="s">
         <v>180</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>181</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>182</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>183</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>184</v>
-      </c>
-      <c r="H2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I2" t="s">
-        <v>186</v>
       </c>
       <c r="J2" t="s">
         <v>4</v>
       </c>
       <c r="K2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L2" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" t="s">
         <v>187</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>188</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" t="s">
         <v>189</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="J3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
       </c>
       <c r="K3">
         <v>24965246.128183831</v>
@@ -1154,19 +1154,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
       </c>
       <c r="K4">
         <v>1288468.9201645069</v>
@@ -1192,19 +1192,19 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="J5" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
       </c>
       <c r="K5">
         <v>230191.46897492089</v>
@@ -1230,19 +1230,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>11</v>
       </c>
       <c r="K6">
         <v>178705.06184309252</v>
@@ -1268,19 +1268,19 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K7">
         <v>97771.835813462851</v>
@@ -1306,19 +1306,19 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>28</v>
       </c>
       <c r="K8">
         <v>466041.10015869705</v>
@@ -1344,19 +1344,19 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K9">
         <v>128250.99022235045</v>
@@ -1382,19 +1382,19 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>33</v>
       </c>
       <c r="K10">
         <v>1736.1153986195452</v>
@@ -1420,19 +1420,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
+      <c r="J11" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" t="s">
-        <v>38</v>
       </c>
       <c r="K11">
         <v>196777.12553570265</v>
@@ -1458,19 +1458,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K12">
         <v>259165.86622702488</v>
@@ -1496,19 +1496,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K13">
         <v>81810.361536814045</v>
@@ -1534,19 +1534,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K14">
         <v>14847.919278129972</v>
@@ -1572,19 +1572,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K15">
         <v>31895.87194649009</v>
@@ -1610,19 +1610,19 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K16">
         <v>42305.282163536431</v>
@@ -1648,19 +1648,19 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <v>118561.91297201814</v>
@@ -1686,19 +1686,19 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K18">
         <v>45833216.792469583</v>
@@ -1724,19 +1724,19 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K19">
         <v>9600.4773434214167</v>
@@ -1762,19 +1762,19 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K20">
         <v>25428190.928034011</v>
@@ -1800,19 +1800,19 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K21">
         <v>85293.345618346313</v>
@@ -1838,19 +1838,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
-      </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K22">
         <v>988.46631917228888</v>
@@ -1876,19 +1876,19 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K23">
         <v>20210717.506183945</v>
@@ -1914,19 +1914,19 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K24">
         <v>2878524.2770361695</v>
@@ -1952,19 +1952,19 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K25">
         <v>589526.73014329805</v>
@@ -1990,19 +1990,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
         <v>72</v>
       </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" t="s">
-        <v>74</v>
-      </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K26">
         <v>7790.9166015573965</v>
@@ -2028,19 +2028,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K27">
         <v>2166428.3608621312</v>
@@ -2066,19 +2066,19 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" t="s">
         <v>77</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" t="s">
-        <v>79</v>
       </c>
       <c r="K28">
         <v>1374527.5713624337</v>
@@ -2104,19 +2104,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>81</v>
       </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>83</v>
-      </c>
       <c r="J29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K29">
         <v>36340.85512554364</v>
@@ -2142,19 +2142,19 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="J30" t="s">
         <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>83</v>
-      </c>
-      <c r="J30" t="s">
-        <v>86</v>
       </c>
       <c r="K30">
         <v>68737.202118534289</v>
@@ -2180,19 +2180,19 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J31" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" t="s">
-        <v>89</v>
       </c>
       <c r="K31">
         <v>100484.3202610756</v>
@@ -2218,19 +2218,19 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>92</v>
-      </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K32">
         <v>14088280.445939962</v>
@@ -2256,19 +2256,19 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K33">
         <v>118941.23272573021</v>
@@ -2294,19 +2294,19 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K34">
         <v>21988.936351392673</v>
@@ -2332,19 +2332,19 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K35">
         <v>11935572.900812317</v>
@@ -2370,19 +2370,19 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" t="s">
         <v>99</v>
       </c>
-      <c r="B36" t="s">
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" t="s">
         <v>100</v>
-      </c>
-      <c r="D36" t="s">
-        <v>101</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" t="s">
-        <v>102</v>
       </c>
       <c r="K36">
         <v>2107.7428559933919</v>
@@ -2408,19 +2408,19 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K37">
         <v>314936.79875185777</v>
@@ -2446,19 +2446,19 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K38">
         <v>91117.578012331389</v>
@@ -2484,19 +2484,19 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" t="s">
         <v>107</v>
-      </c>
-      <c r="B39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" t="s">
-        <v>101</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39" t="s">
-        <v>109</v>
       </c>
       <c r="K39">
         <v>26.865407941423623</v>
@@ -2522,19 +2522,19 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K40">
         <v>1988.9893256430512</v>
@@ -2560,19 +2560,19 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K41">
         <v>116613.16602106349</v>
@@ -2598,19 +2598,19 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K42">
         <v>2641303.9499925142</v>
@@ -2636,19 +2636,19 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" t="s">
         <v>116</v>
       </c>
-      <c r="B43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" t="s">
-        <v>118</v>
-      </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J43" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K43">
         <v>34886.045315286356</v>
@@ -2674,19 +2674,19 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
         <v>119</v>
       </c>
-      <c r="B44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>121</v>
-      </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K44">
         <v>13266889.881567331</v>
@@ -2712,19 +2712,19 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K45">
         <v>1436916.8962362793</v>
@@ -2750,19 +2750,19 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D46" t="s">
-        <v>126</v>
-      </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J46" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K46">
         <v>6611043.5529440343</v>
@@ -2788,19 +2788,19 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" t="s">
         <v>127</v>
       </c>
-      <c r="B47" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" t="s">
-        <v>129</v>
-      </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K47">
         <v>8307064.9522866216</v>
@@ -2826,19 +2826,19 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" t="s">
         <v>130</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="s">
         <v>131</v>
       </c>
-      <c r="D48" t="s">
-        <v>132</v>
-      </c>
-      <c r="E48" t="s">
-        <v>133</v>
-      </c>
       <c r="J48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K48">
         <v>6086.1963717252083</v>
@@ -2864,19 +2864,19 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" t="s">
         <v>134</v>
       </c>
-      <c r="B49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>136</v>
-      </c>
       <c r="E49" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K49">
         <v>121886.58843968091</v>
@@ -2902,19 +2902,19 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" t="s">
         <v>137</v>
       </c>
-      <c r="B50" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" t="s">
-        <v>139</v>
-      </c>
       <c r="E50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J50" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K50">
         <v>3073484.0384656894</v>
@@ -2940,19 +2940,19 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" t="s">
         <v>140</v>
       </c>
-      <c r="B51" t="s">
-        <v>141</v>
-      </c>
-      <c r="D51" t="s">
-        <v>142</v>
-      </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K51">
         <v>244176.80273373649</v>
@@ -2978,19 +2978,19 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" t="s">
         <v>143</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>144</v>
       </c>
-      <c r="D52" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" t="s">
-        <v>146</v>
-      </c>
       <c r="J52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K52">
         <v>240504.60431777878</v>
@@ -3067,10 +3067,10 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
@@ -3081,63 +3081,63 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" t="s">
         <v>171</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>172</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>173</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>174</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M2" t="s">
         <v>175</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N2" t="s">
         <v>176</v>
       </c>
-      <c r="I2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" t="s">
         <v>151</v>
-      </c>
-      <c r="L2" t="s">
-        <v>152</v>
-      </c>
-      <c r="M2" t="s">
-        <v>177</v>
-      </c>
-      <c r="N2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" t="s">
-        <v>179</v>
-      </c>
-      <c r="P2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3169,19 +3169,19 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3214,19 +3214,19 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H5">
         <v>0.6</v>
@@ -3255,19 +3255,19 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
         <v>156</v>
-      </c>
-      <c r="D6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E6" t="s">
-        <v>158</v>
       </c>
       <c r="F6">
         <v>0.95</v>
@@ -3302,19 +3302,19 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" t="s">
         <v>156</v>
-      </c>
-      <c r="D7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" t="s">
-        <v>158</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3349,19 +3349,19 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H9">
         <v>0.8</v>
@@ -3431,19 +3431,19 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3475,19 +3475,19 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3519,19 +3519,19 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3563,16 +3563,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -3604,16 +3604,16 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -3645,16 +3645,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3686,16 +3686,16 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3727,16 +3727,16 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3768,16 +3768,16 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -3809,16 +3809,16 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H19">
         <v>0.12</v>
@@ -3847,16 +3847,16 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H20">
         <v>0.3</v>
@@ -3885,16 +3885,16 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21">
         <v>0.4</v>
@@ -3923,16 +3923,16 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H22">
         <v>0.5</v>
@@ -3961,16 +3961,16 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H23">
         <v>0.6</v>
@@ -3999,16 +3999,16 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H24">
         <v>0.8</v>
@@ -4037,19 +4037,19 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H25">
         <v>0.7</v>
@@ -4078,16 +4078,16 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4119,16 +4119,16 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -4160,19 +4160,19 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F28">
         <v>0.95</v>
@@ -4204,19 +4204,19 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H29">
         <v>0.8</v>
@@ -4239,19 +4239,19 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H30">
         <v>0.9</v>
@@ -4280,16 +4280,16 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F31">
         <v>0.99</v>
@@ -4321,19 +4321,19 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H32">
         <v>0.81</v>
@@ -4362,16 +4362,16 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F33">
         <v>0.85</v>
@@ -4403,16 +4403,16 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -4441,19 +4441,19 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D35" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -4482,16 +4482,16 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4517,16 +4517,16 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -4558,19 +4558,19 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H38">
         <v>0.159</v>
@@ -4599,19 +4599,19 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H39">
         <v>0.75</v>
@@ -4640,16 +4640,16 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -4678,19 +4678,19 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F41">
         <v>0.71</v>
@@ -4716,19 +4716,19 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F42">
         <v>0.75</v>
@@ -4760,19 +4760,19 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4804,16 +4804,16 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E44" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4845,16 +4845,16 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E45" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F45">
         <v>0.86</v>
@@ -4886,16 +4886,16 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E46" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F46">
         <v>0.86</v>
@@ -4927,19 +4927,19 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4971,19 +4971,19 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D48" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -5015,16 +5015,16 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F49">
         <v>0.65</v>
@@ -5056,19 +5056,19 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D50" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F50">
         <v>0.65</v>
@@ -5100,19 +5100,19 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F51">
         <v>0.65</v>
@@ -5147,16 +5147,16 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E52" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -5188,19 +5188,19 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E53" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -5229,19 +5229,19 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -5273,16 +5273,16 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F55">
         <v>0.7</v>
@@ -5314,16 +5314,16 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E56" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -5355,16 +5355,16 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -5396,16 +5396,16 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E58" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F58">
         <v>0.97</v>
@@ -5437,16 +5437,16 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E59" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -5478,19 +5478,19 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D60" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -5522,19 +5522,19 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D61" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F61">
         <v>0.75</v>
@@ -5566,19 +5566,19 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E62" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5610,16 +5610,16 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5651,16 +5651,16 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -5692,16 +5692,16 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E65" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F65">
         <v>0.95</v>
@@ -5733,19 +5733,19 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C66" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E66" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F66">
         <v>0.95</v>
@@ -5777,19 +5777,19 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D67" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F67">
         <v>0.93</v>
@@ -5821,16 +5821,16 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C68" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E68" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -5862,19 +5862,19 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -5906,16 +5906,16 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C70" t="s">
+        <v>160</v>
+      </c>
+      <c r="E70" t="s">
         <v>162</v>
-      </c>
-      <c r="E70" t="s">
-        <v>164</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -5944,16 +5944,16 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E71" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -5985,19 +5985,19 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D72" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -6029,19 +6029,19 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C73" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D73" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E73" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H73">
         <v>0.7</v>
@@ -6070,16 +6070,16 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -6111,19 +6111,19 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B75" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D75" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -6155,16 +6155,16 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C76" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6196,19 +6196,19 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E77" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6240,19 +6240,19 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D78" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6284,19 +6284,19 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D79" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E79" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -6328,16 +6328,16 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E80" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H80">
         <v>0.95</v>
@@ -6366,19 +6366,19 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E81" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6413,19 +6413,19 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D82" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E82" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -6457,19 +6457,19 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B83" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D83" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E83" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -6498,19 +6498,19 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D84" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E84" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H84">
         <v>0.6</v>
@@ -6539,19 +6539,19 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D85" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H85">
         <v>0.95</v>
@@ -6580,16 +6580,16 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B86" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C86" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E86" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -6621,16 +6621,16 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E87" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H87">
         <v>0.89270000000000005</v>
@@ -6659,19 +6659,19 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D88" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E88" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F88">
         <v>0.93100000000000005</v>
@@ -6703,16 +6703,16 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B89" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C89" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E89" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G89">
         <v>0.04</v>
@@ -6741,19 +6741,19 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D90" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E90" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G90">
         <v>0.7</v>
@@ -6782,16 +6782,16 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B91" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C91" t="s">
+        <v>160</v>
+      </c>
+      <c r="E91" t="s">
         <v>162</v>
-      </c>
-      <c r="E91" t="s">
-        <v>164</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -6820,16 +6820,16 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B92" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C92" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E92" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -6858,16 +6858,16 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B93" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C93" t="s">
+        <v>160</v>
+      </c>
+      <c r="E93" t="s">
         <v>162</v>
-      </c>
-      <c r="E93" t="s">
-        <v>164</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -6896,16 +6896,16 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B94" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E94" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G94">
         <v>1</v>
@@ -6934,16 +6934,16 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B95" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C95" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E95" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -6975,16 +6975,16 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E96" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -7016,19 +7016,19 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D97" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E97" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -7060,19 +7060,19 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D98" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E98" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7104,16 +7104,16 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C99" t="s">
+        <v>160</v>
+      </c>
+      <c r="E99" t="s">
         <v>162</v>
-      </c>
-      <c r="E99" t="s">
-        <v>164</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -7142,16 +7142,16 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E100" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -7180,19 +7180,19 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D101" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E101" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F101">
         <v>0.87</v>
@@ -7224,16 +7224,16 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C102" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E102" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -7262,16 +7262,16 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B103" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C103" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E103" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F103">
         <v>0.27</v>
@@ -7303,19 +7303,19 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C104" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D104" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E104" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -7347,19 +7347,19 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C105" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D105" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E105" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -7391,19 +7391,19 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B106" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C106" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D106" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H106">
         <v>0.44</v>
@@ -7432,19 +7432,19 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C107" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D107" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E107" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -7476,16 +7476,16 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B108" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C108" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F108">
         <v>0.94</v>
@@ -7517,16 +7517,16 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B109" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C109" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E109" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F109">
         <v>0.94</v>
@@ -7558,19 +7558,19 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C110" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D110" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F110">
         <v>0.94</v>
@@ -7602,19 +7602,19 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B111" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D111" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E111" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -7643,19 +7643,19 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B112" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C112" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E112" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F112">
         <v>0.99</v>
@@ -7684,16 +7684,16 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C113" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E113" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -7725,19 +7725,19 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D114" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E114" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H114">
         <v>1</v>
@@ -7766,16 +7766,16 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B115" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E115" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F115">
         <v>0.99</v>
@@ -7807,16 +7807,16 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B116" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E116" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -7848,16 +7848,16 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C117" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E117" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F117">
         <v>0.66839999999999999</v>
@@ -7889,19 +7889,19 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B118" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C118" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F118">
         <v>0.2024</v>
@@ -7933,19 +7933,19 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C119" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D119" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E119" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F119">
         <v>0.66900000000000004</v>
@@ -7977,16 +7977,16 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B120" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C120" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E120" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -8018,19 +8018,19 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C121" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D121" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E121" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F121">
         <v>0.6</v>

</xml_diff>